<commit_message>
Cleaned up more styles.
</commit_message>
<xml_diff>
--- a/examples/styles/out.xlsx
+++ b/examples/styles/out.xlsx
@@ -28,6 +28,15 @@
   <si>
     <t>bold</t>
   </si>
+  <si>
+    <t>italic</t>
+  </si>
+  <si>
+    <t>underline</t>
+  </si>
+  <si>
+    <t>strikethrough</t>
+  </si>
 </sst>
 </file>
 
@@ -43,6 +52,15 @@
     </font>
     <font>
       <b/>
+    </font>
+    <font>
+      <i/>
+    </font>
+    <font>
+      <u/>
+    </font>
+    <font>
+      <strike/>
     </font>
   </fonts>
   <fills>
@@ -62,6 +80,9 @@
       <diagonal/>
     </border>
     <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -69,6 +90,9 @@
   <cellXfs>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf fontId="1" borderId="1" applyFont="1" applyBorder="1"/>
+    <xf fontId="2" borderId="2" applyFont="1" applyBorder="1"/>
+    <xf fontId="3" borderId="3" applyFont="1" applyBorder="1"/>
+    <xf fontId="4" borderId="4" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -363,6 +387,21 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="4">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Even more style fixes.
</commit_message>
<xml_diff>
--- a/examples/styles/out.xlsx
+++ b/examples/styles/out.xlsx
@@ -37,6 +37,30 @@
   <si>
     <t>strikethrough</t>
   </si>
+  <si>
+    <t>font vertical alignment</t>
+  </si>
+  <si>
+    <t>superscript</t>
+  </si>
+  <si>
+    <t>subscript</t>
+  </si>
+  <si>
+    <t>larger</t>
+  </si>
+  <si>
+    <t>smaller</t>
+  </si>
+  <si>
+    <t>comic sans</t>
+  </si>
+  <si>
+    <t>rgb font color</t>
+  </si>
+  <si>
+    <t>indexed font color</t>
+  </si>
 </sst>
 </file>
 
@@ -61,6 +85,27 @@
     </font>
     <font>
       <strike/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+    </font>
+    <font>
+      <sz val="14"/>
+    </font>
+    <font>
+      <sz val="8"/>
+    </font>
+    <font>
+      <name val="Comic Sans MS"/>
+    </font>
+    <font>
+      <color indexed="4"/>
     </font>
   </fonts>
   <fills>
@@ -83,6 +128,13 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -93,6 +145,13 @@
     <xf fontId="2" borderId="2" applyFont="1" applyBorder="1"/>
     <xf fontId="3" borderId="3" applyFont="1" applyBorder="1"/>
     <xf fontId="4" borderId="4" applyFont="1" applyBorder="1"/>
+    <xf fontId="5" borderId="5" applyFont="1" applyBorder="1"/>
+    <xf fontId="6" borderId="6" applyFont="1" applyBorder="1"/>
+    <xf fontId="7" borderId="7" applyFont="1" applyBorder="1"/>
+    <xf fontId="8" borderId="8" applyFont="1" applyBorder="1"/>
+    <xf fontId="9" borderId="9" applyFont="1" applyBorder="1"/>
+    <xf fontId="10" borderId="10" applyFont="1" applyBorder="1"/>
+    <xf fontId="11" borderId="11" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,6 +461,41 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added double underline support.
</commit_message>
<xml_diff>
--- a/examples/styles/out.xlsx
+++ b/examples/styles/out.xlsx
@@ -35,6 +35,9 @@
     <t>underline</t>
   </si>
   <si>
+    <t>double underline</t>
+  </si>
+  <si>
     <t>strikethrough</t>
   </si>
   <si>
@@ -124,6 +127,9 @@
     </font>
     <font>
       <u/>
+    </font>
+    <font>
+      <u val="double"/>
     </font>
     <font>
       <strike/>
@@ -209,6 +215,7 @@
     <border/>
     <border/>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -226,45 +233,46 @@
     <xf fontId="9" borderId="9" applyFont="1" applyBorder="1"/>
     <xf fontId="10" borderId="10" applyFont="1" applyBorder="1"/>
     <xf fontId="11" borderId="11" applyFont="1" applyBorder="1"/>
-    <xf fontId="12" borderId="12" applyFont="1" applyBorder="1">
+    <xf fontId="12" borderId="12" applyFont="1" applyBorder="1"/>
+    <xf fontId="13" borderId="13" applyFont="1" applyBorder="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="13" borderId="13" applyFont="1" applyBorder="1">
+    <xf fontId="14" borderId="14" applyFont="1" applyBorder="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf fontId="14" borderId="14" applyFont="1" applyBorder="1">
+    <xf fontId="15" borderId="15" applyFont="1" applyBorder="1">
       <alignment vertical="top"/>
     </xf>
-    <xf fontId="15" borderId="15" applyFont="1" applyBorder="1">
+    <xf fontId="16" borderId="16" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf fontId="16" borderId="16" applyFont="1" applyBorder="1">
+    <xf fontId="17" borderId="17" applyFont="1" applyBorder="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf fontId="17" borderId="17" applyFont="1" applyBorder="1">
+    <xf fontId="18" borderId="18" applyFont="1" applyBorder="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf fontId="18" borderId="18" applyFont="1" applyBorder="1"/>
     <xf fontId="19" borderId="19" applyFont="1" applyBorder="1"/>
-    <xf fontId="20" borderId="20" applyFont="1" applyBorder="1">
+    <xf fontId="20" borderId="20" applyFont="1" applyBorder="1"/>
+    <xf fontId="21" borderId="21" applyFont="1" applyBorder="1">
       <alignment indent="2"/>
     </xf>
-    <xf fontId="21" borderId="21" applyFont="1" applyBorder="1">
+    <xf fontId="22" borderId="22" applyFont="1" applyBorder="1">
       <alignment textRotation="20"/>
     </xf>
-    <xf fontId="22" borderId="22" applyFont="1" applyBorder="1">
+    <xf fontId="23" borderId="23" applyFont="1" applyBorder="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf fontId="23" borderId="23" applyFont="1" applyBorder="1">
+    <xf fontId="24" borderId="24" applyFont="1" applyBorder="1">
       <alignment textRotation="135"/>
     </xf>
-    <xf fontId="24" borderId="24" applyFont="1" applyBorder="1">
+    <xf fontId="25" borderId="25" applyFont="1" applyBorder="1">
       <alignment textRotation="255"/>
     </xf>
-    <xf fontId="25" borderId="25" applyFont="1" applyBorder="1">
+    <xf fontId="26" borderId="26" applyFont="1" applyBorder="1">
       <alignment textRotation="90"/>
     </xf>
-    <xf fontId="26" borderId="26" applyFont="1" applyBorder="1">
+    <xf fontId="27" borderId="27" applyFont="1" applyBorder="1">
       <alignment textRotation="180"/>
     </xf>
   </cellXfs>
@@ -641,8 +649,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="s" s="18">
+    <row r="18">
+      <c r="A18" t="s" s="18">
         <v>17</v>
       </c>
     </row>
@@ -651,8 +659,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" t="s" s="20">
+    <row r="21">
+      <c r="A21" t="s" s="20">
         <v>19</v>
       </c>
     </row>
@@ -684,6 +692,11 @@
     <row r="34">
       <c r="A34" t="s" s="26">
         <v>25</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="27">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reworked style example a bit.
</commit_message>
<xml_diff>
--- a/examples/styles/out.xlsx
+++ b/examples/styles/out.xlsx
@@ -339,7 +339,9 @@
     <xf fontId="9" borderId="9" applyFont="1" applyBorder="1"/>
     <xf fontId="10" borderId="10" applyFont="1" applyBorder="1"/>
     <xf fontId="11" borderId="11" applyFont="1" applyBorder="1"/>
-    <xf fontId="12" borderId="12" applyFont="1" applyBorder="1"/>
+    <xf fontId="12" borderId="12" applyFont="1" applyBorder="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf fontId="13" borderId="13" applyFont="1" applyBorder="1">
       <alignment horizontal="center"/>
     </xf>
@@ -685,6 +687,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -777,6 +780,9 @@
         <v>17</v>
       </c>
     </row>
+    <row r="19">
+      <c r="A19"/>
+    </row>
     <row r="20">
       <c r="A20" t="s" s="19">
         <v>18</v>

</xml_diff>

<commit_message>
Reworked StyleSheet to use JSON.
</commit_message>
<xml_diff>
--- a/examples/styles/out.xlsx
+++ b/examples/styles/out.xlsx
@@ -169,7 +169,7 @@
     <numFmt numFmtId="167" formatCode="[$-x-sysdate]dddd, mmmm dd, yyyy"/>
     <numFmt numFmtId="168" formatCode="[$-x-systime]h:mm:ss AM/PM"/>
   </numFmts>
-  <fonts count="45" x14ac:knownFonts="1">
+  <fonts x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,7 +184,7 @@
       <i/>
     </font>
     <font>
-      <u/>
+      <strike/>
     </font>
     <font>
       <u val="double"/>
@@ -248,7 +248,7 @@
     <font/>
     <font/>
   </fonts>
-  <fills count="46">
+  <fills>
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -300,7 +300,7 @@
     <fill/>
     <fill/>
   </fills>
-  <borders count="45">
+  <borders>
     <border>
       <left/>
       <right/>
@@ -370,7 +370,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf fontId="1" fillId="2" borderId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="2" fillId="3" borderId="2" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -402,7 +402,7 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf fontId="18" fillId="19" borderId="18" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment wrapText="1"/>
+      <alignment wrapText="true"/>
     </xf>
     <xf fontId="19" fillId="20" borderId="19" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="20" fillId="21" borderId="20" applyFont="1" applyFill="1" applyBorder="1"/>

</xml_diff>

<commit_message>
Have fills basically functioning.
</commit_message>
<xml_diff>
--- a/examples/styles/out.xlsx
+++ b/examples/styles/out.xlsx
@@ -86,6 +86,9 @@
     <t>right-to-right</t>
   </si>
   <si>
+    <t>background color</t>
+  </si>
+  <si>
     <t>rgb font color</t>
   </si>
   <si>
@@ -223,11 +226,12 @@
     <font/>
     <font/>
     <font/>
+    <font/>
     <font>
       <color rgb="ff0000"/>
     </font>
     <font>
-      <color indexed="4"/>
+      <color theme="4"/>
     </font>
     <font/>
     <font/>
@@ -281,6 +285,11 @@
     <fill/>
     <fill/>
     <fill/>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ff0000"/>
+      </patternFill>
+    </fill>
     <fill/>
     <fill/>
     <fill/>
@@ -316,6 +325,7 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
     <border/>
     <border/>
     <border/>
@@ -431,37 +441,38 @@
     <xf fontId="27" fillId="28" borderId="27" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="28" fillId="29" borderId="28" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="29" fillId="30" borderId="29" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="30" fillId="31" borderId="30" applyFont="1" applyFill="1" applyBorder="1">
+    <xf fontId="30" fillId="31" borderId="30" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="31" fillId="32" borderId="31" applyFont="1" applyFill="1" applyBorder="1">
       <alignment indent="2"/>
     </xf>
-    <xf fontId="31" fillId="32" borderId="31" applyFont="1" applyFill="1" applyBorder="1">
+    <xf fontId="32" fillId="33" borderId="32" applyFont="1" applyFill="1" applyBorder="1">
       <alignment textRotation="20"/>
     </xf>
-    <xf fontId="32" fillId="33" borderId="32" applyFont="1" applyFill="1" applyBorder="1">
+    <xf fontId="33" fillId="34" borderId="33" applyFont="1" applyFill="1" applyBorder="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf fontId="33" fillId="34" borderId="33" applyFont="1" applyFill="1" applyBorder="1">
+    <xf fontId="34" fillId="35" borderId="34" applyFont="1" applyFill="1" applyBorder="1">
       <alignment textRotation="135"/>
     </xf>
-    <xf fontId="34" fillId="35" borderId="34" applyFont="1" applyFill="1" applyBorder="1">
+    <xf fontId="35" fillId="36" borderId="35" applyFont="1" applyFill="1" applyBorder="1">
       <alignment textRotation="255"/>
     </xf>
-    <xf fontId="35" fillId="36" borderId="35" applyFont="1" applyFill="1" applyBorder="1">
+    <xf fontId="36" fillId="37" borderId="36" applyFont="1" applyFill="1" applyBorder="1">
       <alignment textRotation="90"/>
     </xf>
-    <xf fontId="36" fillId="37" borderId="36" applyFont="1" applyFill="1" applyBorder="1">
+    <xf fontId="37" fillId="38" borderId="37" applyFont="1" applyFill="1" applyBorder="1">
       <alignment textRotation="180"/>
     </xf>
-    <xf fontId="37" fillId="38" borderId="37" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2"/>
-    <xf fontId="38" fillId="39" borderId="38" applyFont="1" applyFill="1" applyBorder="1" numFmtId="164"/>
-    <xf fontId="39" fillId="40" borderId="39" applyFont="1" applyFill="1" applyBorder="1" numFmtId="165"/>
-    <xf fontId="40" fillId="41" borderId="40" applyFont="1" applyFill="1" applyBorder="1" numFmtId="166"/>
-    <xf fontId="41" fillId="42" borderId="41" applyFont="1" applyFill="1" applyBorder="1" numFmtId="167"/>
-    <xf fontId="42" fillId="43" borderId="42" applyFont="1" applyFill="1" applyBorder="1" numFmtId="168"/>
-    <xf fontId="43" fillId="44" borderId="43" applyFont="1" applyFill="1" applyBorder="1" numFmtId="10"/>
-    <xf fontId="44" fillId="45" borderId="44" applyFont="1" applyFill="1" applyBorder="1" numFmtId="12"/>
-    <xf fontId="45" fillId="46" borderId="45" applyFont="1" applyFill="1" applyBorder="1" numFmtId="11"/>
-    <xf fontId="46" fillId="47" borderId="46" applyFont="1" applyFill="1" applyBorder="1" numFmtId="49"/>
+    <xf fontId="38" fillId="39" borderId="38" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2"/>
+    <xf fontId="39" fillId="40" borderId="39" applyFont="1" applyFill="1" applyBorder="1" numFmtId="164"/>
+    <xf fontId="40" fillId="41" borderId="40" applyFont="1" applyFill="1" applyBorder="1" numFmtId="165"/>
+    <xf fontId="41" fillId="42" borderId="41" applyFont="1" applyFill="1" applyBorder="1" numFmtId="166"/>
+    <xf fontId="42" fillId="43" borderId="42" applyFont="1" applyFill="1" applyBorder="1" numFmtId="167"/>
+    <xf fontId="43" fillId="44" borderId="43" applyFont="1" applyFill="1" applyBorder="1" numFmtId="168"/>
+    <xf fontId="44" fillId="45" borderId="44" applyFont="1" applyFill="1" applyBorder="1" numFmtId="10"/>
+    <xf fontId="45" fillId="46" borderId="45" applyFont="1" applyFill="1" applyBorder="1" numFmtId="12"/>
+    <xf fontId="46" fillId="47" borderId="46" applyFont="1" applyFill="1" applyBorder="1" numFmtId="11"/>
+    <xf fontId="47" fillId="48" borderId="47" applyFont="1" applyFill="1" applyBorder="1" numFmtId="49"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -853,165 +864,167 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21"/>
+      <c r="A21" t="s" s="21">
+        <v>20</v>
+      </c>
     </row>
     <row r="22">
-      <c r="A22" t="s" s="21">
-        <v>20</v>
+      <c r="A22" t="s" s="22">
+        <v>21</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="s" s="22">
-        <v>21</v>
+      <c r="A23" t="s" s="23">
+        <v>22</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="s" s="23">
-        <v>22</v>
+      <c r="A24" t="s" s="24">
+        <v>23</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="s" s="24">
-        <v>23</v>
+      <c r="A25" t="s" s="25">
+        <v>24</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="s" s="25">
-        <v>24</v>
+      <c r="A26" t="s" s="26">
+        <v>25</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="s" s="26">
-        <v>25</v>
+      <c r="A27" t="s" s="27">
+        <v>26</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="s" s="27">
-        <v>26</v>
+      <c r="A28" t="s" s="28">
+        <v>27</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="s" s="28">
-        <v>27</v>
+      <c r="A29" t="s" s="29">
+        <v>28</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="s" s="29">
-        <v>28</v>
+      <c r="A30" t="s" s="30">
+        <v>29</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="s" s="30">
-        <v>29</v>
+      <c r="A31" t="s" s="31">
+        <v>30</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="s" s="31">
-        <v>30</v>
+      <c r="A32" t="s" s="32">
+        <v>31</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="s" s="32">
-        <v>31</v>
+      <c r="A33" t="s" s="33">
+        <v>32</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="s" s="33">
-        <v>32</v>
+      <c r="A34" t="s" s="34">
+        <v>33</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="s" s="34">
-        <v>33</v>
+      <c r="A35" t="s" s="35">
+        <v>34</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="s" s="35">
-        <v>34</v>
+      <c r="A36" t="s" s="36">
+        <v>35</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="s" s="36">
-        <v>35</v>
+      <c r="A37" t="s" s="37">
+        <v>36</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>36</v>
-      </c>
-      <c r="B38" s="37">
+        <v>37</v>
+      </c>
+      <c r="B38" s="38">
         <v>1.2</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>37</v>
-      </c>
-      <c r="B39" s="38">
+        <v>38</v>
+      </c>
+      <c r="B39" s="39">
         <v>1.2</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>38</v>
-      </c>
-      <c r="B40" s="39">
+        <v>39</v>
+      </c>
+      <c r="B40" s="40">
         <v>1.2</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>39</v>
-      </c>
-      <c r="B41" s="40">
+        <v>40</v>
+      </c>
+      <c r="B41" s="41">
         <v>1.2</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>40</v>
-      </c>
-      <c r="B42" s="41">
+        <v>41</v>
+      </c>
+      <c r="B42" s="42">
         <v>1.2</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>41</v>
-      </c>
-      <c r="B43" s="42">
+        <v>42</v>
+      </c>
+      <c r="B43" s="43">
         <v>1.2</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>42</v>
-      </c>
-      <c r="B44" s="43">
+        <v>43</v>
+      </c>
+      <c r="B44" s="44">
         <v>1.2</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>43</v>
-      </c>
-      <c r="B45" s="44">
+        <v>44</v>
+      </c>
+      <c r="B45" s="45">
         <v>1.2</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>44</v>
-      </c>
-      <c r="B46" s="45">
+        <v>45</v>
+      </c>
+      <c r="B46" s="46">
         <v>1.2</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>45</v>
-      </c>
-      <c r="B47" s="46">
+        <v>46</v>
+      </c>
+      <c r="B47" s="47">
         <v>1.2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added more _Style tests.
</commit_message>
<xml_diff>
--- a/examples/styles/out.xlsx
+++ b/examples/styles/out.xlsx
@@ -56,22 +56,25 @@
     <t>comic sans</t>
   </si>
   <si>
-    <t>left</t>
-  </si>
-  <si>
-    <t>center</t>
-  </si>
-  <si>
-    <t>right</t>
-  </si>
-  <si>
-    <t>top</t>
-  </si>
-  <si>
-    <t>middle</t>
-  </si>
-  <si>
-    <t>bottom</t>
+    <t>rgb font color</t>
+  </si>
+  <si>
+    <t>theme font color</t>
+  </si>
+  <si>
+    <t>tinted theme font color</t>
+  </si>
+  <si>
+    <t>horizontal center</t>
+  </si>
+  <si>
+    <t>this text is justified distributed</t>
+  </si>
+  <si>
+    <t>indent</t>
+  </si>
+  <si>
+    <t>vertical center</t>
   </si>
   <si>
     <t>this text is wrapped text</t>
@@ -80,21 +83,30 @@
     <t>this text is shrink to fit</t>
   </si>
   <si>
-    <t>left-to-right</t>
-  </si>
-  <si>
-    <t>right-to-right</t>
+    <t>right-to-left</t>
+  </si>
+  <si>
+    <t>text rotation</t>
+  </si>
+  <si>
+    <t>angle counterclockwise</t>
+  </si>
+  <si>
+    <t>angle clockwise</t>
+  </si>
+  <si>
+    <t>verticalText</t>
+  </si>
+  <si>
+    <t>rotate text up</t>
+  </si>
+  <si>
+    <t>rotate text down</t>
   </si>
   <si>
     <t>background color</t>
   </si>
   <si>
-    <t>rgb font color</t>
-  </si>
-  <si>
-    <t>indexed font color</t>
-  </si>
-  <si>
     <t>top border</t>
   </si>
   <si>
@@ -114,27 +126,6 @@
   </si>
   <si>
     <t>thick bottom border</t>
-  </si>
-  <si>
-    <t>indent</t>
-  </si>
-  <si>
-    <t>text rotation</t>
-  </si>
-  <si>
-    <t>angle counterclockwise</t>
-  </si>
-  <si>
-    <t>angle clockwise</t>
-  </si>
-  <si>
-    <t>verticalText</t>
-  </si>
-  <si>
-    <t>rotate text up</t>
-  </si>
-  <si>
-    <t>rotate text down</t>
   </si>
   <si>
     <t>number</t>
@@ -216,23 +207,22 @@
     <font>
       <name val="Comic Sans MS"/>
     </font>
-    <font/>
-    <font/>
-    <font/>
-    <font/>
-    <font/>
-    <font/>
-    <font/>
-    <font/>
-    <font/>
-    <font/>
-    <font/>
-    <font>
-      <color rgb="ff0000"/>
+    <font>
+      <color rgb="FF0000"/>
     </font>
     <font>
       <color theme="4"/>
     </font>
+    <font>
+      <color theme="4" tint="-0.5"/>
+    </font>
+    <font/>
+    <font/>
+    <font/>
+    <font/>
+    <font/>
+    <font/>
+    <font/>
     <font/>
     <font/>
     <font/>
@@ -285,20 +275,17 @@
     <fill/>
     <fill/>
     <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="ff0000"/>
       </patternFill>
     </fill>
-    <fill/>
-    <fill/>
-    <fill/>
-    <fill/>
-    <fill/>
-    <fill/>
-    <fill/>
-    <fill/>
-    <fill/>
     <fill/>
     <fill/>
     <fill/>
@@ -325,6 +312,10 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
     <border/>
     <border/>
     <border/>
@@ -379,13 +370,6 @@
     <border/>
     <border/>
     <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -402,77 +386,66 @@
     <xf fontId="8" fillId="9" borderId="8" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="9" fillId="10" borderId="9" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="10" fillId="11" borderId="10" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="11" fillId="12" borderId="11" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf fontId="12" fillId="13" borderId="12" applyFont="1" applyFill="1" applyBorder="1">
+    <xf fontId="11" fillId="12" borderId="11" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="12" fillId="13" borderId="12" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="13" fillId="14" borderId="13" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="14" fillId="15" borderId="14" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="13" fillId="14" borderId="13" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf fontId="14" fillId="15" borderId="14" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf fontId="15" fillId="16" borderId="15" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="distributed" justifyLastLine="1"/>
+    </xf>
+    <xf fontId="16" fillId="17" borderId="16" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment indent="2"/>
+    </xf>
+    <xf fontId="17" fillId="18" borderId="17" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf fontId="16" fillId="17" borderId="16" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf fontId="17" fillId="18" borderId="17" applyFont="1" applyFill="1" applyBorder="1">
+    <xf fontId="18" fillId="19" borderId="18" applyFont="1" applyFill="1" applyBorder="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf fontId="18" fillId="19" borderId="18" applyFont="1" applyFill="1" applyBorder="1">
+    <xf fontId="19" fillId="20" borderId="19" applyFont="1" applyFill="1" applyBorder="1">
       <alignment shrinkToFit="1"/>
-    </xf>
-    <xf fontId="19" fillId="20" borderId="19" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment readingOrder="1"/>
     </xf>
     <xf fontId="20" fillId="21" borderId="20" applyFont="1" applyFill="1" applyBorder="1">
       <alignment readingOrder="2"/>
     </xf>
-    <xf fontId="21" fillId="22" borderId="21" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="22" fillId="23" borderId="22" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="23" fillId="24" borderId="23" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="24" fillId="25" borderId="24" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="25" fillId="26" borderId="25" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="26" fillId="27" borderId="26" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="21" fillId="22" borderId="21" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment textRotation="100"/>
+    </xf>
+    <xf fontId="22" fillId="23" borderId="22" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf fontId="23" fillId="24" borderId="23" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment textRotation="135"/>
+    </xf>
+    <xf fontId="24" fillId="25" borderId="24" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment textRotation="255"/>
+    </xf>
+    <xf fontId="25" fillId="26" borderId="25" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf fontId="26" fillId="27" borderId="26" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment textRotation="180"/>
+    </xf>
     <xf fontId="27" fillId="28" borderId="27" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="28" fillId="29" borderId="28" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="29" fillId="30" borderId="29" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="30" fillId="31" borderId="30" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="31" fillId="32" borderId="31" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment indent="2"/>
-    </xf>
-    <xf fontId="32" fillId="33" borderId="32" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment textRotation="20"/>
-    </xf>
-    <xf fontId="33" fillId="34" borderId="33" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment textRotation="45"/>
-    </xf>
-    <xf fontId="34" fillId="35" borderId="34" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment textRotation="135"/>
-    </xf>
-    <xf fontId="35" fillId="36" borderId="35" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment textRotation="255"/>
-    </xf>
-    <xf fontId="36" fillId="37" borderId="36" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment textRotation="90"/>
-    </xf>
-    <xf fontId="37" fillId="38" borderId="37" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment textRotation="180"/>
-    </xf>
-    <xf fontId="38" fillId="39" borderId="38" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2"/>
-    <xf fontId="39" fillId="40" borderId="39" applyFont="1" applyFill="1" applyBorder="1" numFmtId="164"/>
-    <xf fontId="40" fillId="41" borderId="40" applyFont="1" applyFill="1" applyBorder="1" numFmtId="165"/>
-    <xf fontId="41" fillId="42" borderId="41" applyFont="1" applyFill="1" applyBorder="1" numFmtId="166"/>
-    <xf fontId="42" fillId="43" borderId="42" applyFont="1" applyFill="1" applyBorder="1" numFmtId="167"/>
-    <xf fontId="43" fillId="44" borderId="43" applyFont="1" applyFill="1" applyBorder="1" numFmtId="168"/>
-    <xf fontId="44" fillId="45" borderId="44" applyFont="1" applyFill="1" applyBorder="1" numFmtId="10"/>
-    <xf fontId="45" fillId="46" borderId="45" applyFont="1" applyFill="1" applyBorder="1" numFmtId="12"/>
-    <xf fontId="46" fillId="47" borderId="46" applyFont="1" applyFill="1" applyBorder="1" numFmtId="11"/>
-    <xf fontId="47" fillId="48" borderId="47" applyFont="1" applyFill="1" applyBorder="1" numFmtId="49"/>
+    <xf fontId="31" fillId="32" borderId="31" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="32" fillId="33" borderId="32" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="33" fillId="34" borderId="33" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="34" fillId="35" borderId="34" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="35" fillId="36" borderId="35" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2"/>
+    <xf fontId="36" fillId="37" borderId="36" applyFont="1" applyFill="1" applyBorder="1" numFmtId="164"/>
+    <xf fontId="37" fillId="38" borderId="37" applyFont="1" applyFill="1" applyBorder="1" numFmtId="165"/>
+    <xf fontId="38" fillId="39" borderId="38" applyFont="1" applyFill="1" applyBorder="1" numFmtId="166"/>
+    <xf fontId="39" fillId="40" borderId="39" applyFont="1" applyFill="1" applyBorder="1" numFmtId="167"/>
+    <xf fontId="40" fillId="41" borderId="40" applyFont="1" applyFill="1" applyBorder="1" numFmtId="168"/>
+    <xf fontId="41" fillId="42" borderId="41" applyFont="1" applyFill="1" applyBorder="1" numFmtId="10"/>
+    <xf fontId="42" fillId="43" borderId="42" applyFont="1" applyFill="1" applyBorder="1" numFmtId="12"/>
+    <xf fontId="43" fillId="44" borderId="43" applyFont="1" applyFill="1" applyBorder="1" numFmtId="11"/>
+    <xf fontId="44" fillId="45" borderId="44" applyFont="1" applyFill="1" applyBorder="1" numFmtId="49"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -934,18 +907,27 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="s" s="35">
+      <c r="A35" t="s">
         <v>34</v>
       </c>
+      <c r="B35" s="35">
+        <v>1.2</v>
+      </c>
     </row>
     <row r="36">
-      <c r="A36" t="s" s="36">
+      <c r="A36" t="s">
         <v>35</v>
       </c>
+      <c r="B36" s="36">
+        <v>1.2</v>
+      </c>
     </row>
     <row r="37">
-      <c r="A37" t="s" s="37">
+      <c r="A37" t="s">
         <v>36</v>
+      </c>
+      <c r="B37" s="37">
+        <v>1.2</v>
       </c>
     </row>
     <row r="38">
@@ -1001,30 +983,6 @@
         <v>43</v>
       </c>
       <c r="B44" s="44">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="s">
-        <v>44</v>
-      </c>
-      <c r="B45" s="45">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="s">
-        <v>45</v>
-      </c>
-      <c r="B46" s="46">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="s">
-        <v>46</v>
-      </c>
-      <c r="B47" s="47">
         <v>1.2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactored get/set fill and tested it.
</commit_message>
<xml_diff>
--- a/examples/styles/out.xlsx
+++ b/examples/styles/out.xlsx
@@ -95,37 +95,52 @@
     <t>angle clockwise</t>
   </si>
   <si>
+    <t>rotate text up</t>
+  </si>
+  <si>
+    <t>rotate text down</t>
+  </si>
+  <si>
     <t>verticalText</t>
   </si>
   <si>
-    <t>rotate text up</t>
-  </si>
-  <si>
-    <t>rotate text down</t>
-  </si>
-  <si>
-    <t>background color</t>
-  </si>
-  <si>
-    <t>top border</t>
-  </si>
-  <si>
-    <t>left border</t>
-  </si>
-  <si>
-    <t>right border</t>
-  </si>
-  <si>
-    <t>bottom border</t>
-  </si>
-  <si>
-    <t>double bottom border</t>
-  </si>
-  <si>
-    <t>medium bottom border</t>
-  </si>
-  <si>
-    <t>thick bottom border</t>
+    <t>rgb solid fill</t>
+  </si>
+  <si>
+    <t>theme solid fill</t>
+  </si>
+  <si>
+    <t>tinted theme solid fill</t>
+  </si>
+  <si>
+    <t>pattern fill</t>
+  </si>
+  <si>
+    <t>linear gradient fill</t>
+  </si>
+  <si>
+    <t>path gradient fill</t>
+  </si>
+  <si>
+    <t>thin border</t>
+  </si>
+  <si>
+    <t>thick border</t>
+  </si>
+  <si>
+    <t>right red border</t>
+  </si>
+  <si>
+    <t>theme diagonal up border</t>
+  </si>
+  <si>
+    <t>various styles border</t>
+  </si>
+  <si>
+    <t>various colors border</t>
+  </si>
+  <si>
+    <t>complex border</t>
   </si>
   <si>
     <t>number</t>
@@ -247,6 +262,11 @@
     <font/>
     <font/>
     <font/>
+    <font/>
+    <font/>
+    <font/>
+    <font/>
+    <font/>
   </fonts>
   <fills>
     <fill>
@@ -283,8 +303,47 @@
     <fill/>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="ff0000"/>
+        <fgColor rgb="FF0000"/>
       </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.25"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="darkDown">
+        <fgColor rgb="FF0000"/>
+        <bgColor theme="3" tint="0.4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <gradientFill degree="10">
+        <stop position="0">
+          <color rgb="FF0000"/>
+        </stop>
+        <stop position="0.5">
+          <color rgb="00FF00"/>
+        </stop>
+        <stop position="1">
+          <color rgb="0000FF"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill type="path" left="0.1" right="0.3" top="0.5" bottom="0.7">
+        <stop position="0">
+          <color rgb="FF0000"/>
+        </stop>
+        <stop position="1">
+          <color rgb="0000FF"/>
+        </stop>
+      </gradientFill>
     </fill>
     <fill/>
     <fill/>
@@ -339,26 +398,75 @@
     <border/>
     <border/>
     <border/>
-    <border>
-      <top style="thin"/>
-    </border>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
     <border>
       <left style="thin"/>
-    </border>
-    <border>
       <right style="thin"/>
-    </border>
-    <border>
+      <top style="thin"/>
       <bottom style="thin"/>
     </border>
     <border>
-      <bottom style="double"/>
+      <left style="thick"/>
+      <right style="thick"/>
+      <top style="thick"/>
+      <bottom style="thick"/>
     </border>
     <border>
+      <left>
+        <color rgb="ff0000"/>
+      </left>
+      <right style="thin">
+        <color rgb="ff0000"/>
+      </right>
+      <top>
+        <color rgb="ff0000"/>
+      </top>
+      <bottom>
+        <color rgb="ff0000"/>
+      </bottom>
+      <diagonal>
+        <color rgb="ff0000"/>
+      </diagonal>
+    </border>
+    <border diagonalUp="1">
+      <diagonal style="dashed">
+        <color theme="6" tint="-0.1"/>
+      </diagonal>
+    </border>
+    <border>
+      <left style="thick"/>
+      <right style="thin"/>
+      <top style="hair"/>
       <bottom style="medium"/>
     </border>
     <border>
-      <bottom style="thick"/>
+      <left style="thick">
+        <color rgb="ffff00"/>
+      </left>
+      <right style="thick">
+        <color rgb="00ff00"/>
+      </right>
+      <top style="thick">
+        <color rgb="ff0000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="0000ff"/>
+      </bottom>
+    </border>
+    <border diagonalUp="1" diagonalDown="1">
+      <left style="mediumDashed"/>
+      <right style="thick"/>
+      <top style="thin"/>
+      <bottom style="dotted">
+        <color rgb="ff0000"/>
+      </bottom>
+      <diagonal style="thick">
+        <color rgb="0000ff"/>
+      </diagonal>
     </border>
     <border/>
     <border/>
@@ -420,13 +528,13 @@
       <alignment textRotation="135"/>
     </xf>
     <xf fontId="24" fillId="25" borderId="24" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf fontId="25" fillId="26" borderId="25" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment textRotation="180"/>
+    </xf>
+    <xf fontId="26" fillId="27" borderId="26" applyFont="1" applyFill="1" applyBorder="1">
       <alignment textRotation="255"/>
-    </xf>
-    <xf fontId="25" fillId="26" borderId="25" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment textRotation="90"/>
-    </xf>
-    <xf fontId="26" fillId="27" borderId="26" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment textRotation="180"/>
     </xf>
     <xf fontId="27" fillId="28" borderId="27" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="28" fillId="29" borderId="28" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -436,16 +544,21 @@
     <xf fontId="32" fillId="33" borderId="32" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="33" fillId="34" borderId="33" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="34" fillId="35" borderId="34" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="35" fillId="36" borderId="35" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2"/>
-    <xf fontId="36" fillId="37" borderId="36" applyFont="1" applyFill="1" applyBorder="1" numFmtId="164"/>
-    <xf fontId="37" fillId="38" borderId="37" applyFont="1" applyFill="1" applyBorder="1" numFmtId="165"/>
-    <xf fontId="38" fillId="39" borderId="38" applyFont="1" applyFill="1" applyBorder="1" numFmtId="166"/>
-    <xf fontId="39" fillId="40" borderId="39" applyFont="1" applyFill="1" applyBorder="1" numFmtId="167"/>
-    <xf fontId="40" fillId="41" borderId="40" applyFont="1" applyFill="1" applyBorder="1" numFmtId="168"/>
-    <xf fontId="41" fillId="42" borderId="41" applyFont="1" applyFill="1" applyBorder="1" numFmtId="10"/>
-    <xf fontId="42" fillId="43" borderId="42" applyFont="1" applyFill="1" applyBorder="1" numFmtId="12"/>
-    <xf fontId="43" fillId="44" borderId="43" applyFont="1" applyFill="1" applyBorder="1" numFmtId="11"/>
-    <xf fontId="44" fillId="45" borderId="44" applyFont="1" applyFill="1" applyBorder="1" numFmtId="49"/>
+    <xf fontId="35" fillId="36" borderId="35" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="36" fillId="37" borderId="36" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="37" fillId="38" borderId="37" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="38" fillId="39" borderId="38" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="39" fillId="40" borderId="39" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="40" fillId="41" borderId="40" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2"/>
+    <xf fontId="41" fillId="42" borderId="41" applyFont="1" applyFill="1" applyBorder="1" numFmtId="164"/>
+    <xf fontId="42" fillId="43" borderId="42" applyFont="1" applyFill="1" applyBorder="1" numFmtId="165"/>
+    <xf fontId="43" fillId="44" borderId="43" applyFont="1" applyFill="1" applyBorder="1" numFmtId="166"/>
+    <xf fontId="44" fillId="45" borderId="44" applyFont="1" applyFill="1" applyBorder="1" numFmtId="167"/>
+    <xf fontId="45" fillId="46" borderId="45" applyFont="1" applyFill="1" applyBorder="1" numFmtId="168"/>
+    <xf fontId="46" fillId="47" borderId="46" applyFont="1" applyFill="1" applyBorder="1" numFmtId="10"/>
+    <xf fontId="47" fillId="48" borderId="47" applyFont="1" applyFill="1" applyBorder="1" numFmtId="12"/>
+    <xf fontId="48" fillId="49" borderId="48" applyFont="1" applyFill="1" applyBorder="1" numFmtId="11"/>
+    <xf fontId="49" fillId="50" borderId="49" applyFont="1" applyFill="1" applyBorder="1" numFmtId="49"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -907,43 +1020,28 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="s">
+      <c r="A35" t="s" s="35">
         <v>34</v>
       </c>
-      <c r="B35" s="35">
-        <v>1.2</v>
-      </c>
     </row>
     <row r="36">
-      <c r="A36" t="s">
+      <c r="A36" t="s" s="36">
         <v>35</v>
       </c>
-      <c r="B36" s="36">
-        <v>1.2</v>
-      </c>
     </row>
     <row r="37">
-      <c r="A37" t="s">
+      <c r="A37" t="s" s="37">
         <v>36</v>
       </c>
-      <c r="B37" s="37">
-        <v>1.2</v>
-      </c>
     </row>
     <row r="38">
-      <c r="A38" t="s">
+      <c r="A38" t="s" s="38">
         <v>37</v>
       </c>
-      <c r="B38" s="38">
-        <v>1.2</v>
-      </c>
     </row>
     <row r="39">
-      <c r="A39" t="s">
+      <c r="A39" t="s" s="39">
         <v>38</v>
-      </c>
-      <c r="B39" s="39">
-        <v>1.2</v>
       </c>
     </row>
     <row r="40">
@@ -983,6 +1081,46 @@
         <v>43</v>
       </c>
       <c r="B44" s="44">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" s="45">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" s="46">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47" s="47">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" s="48">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49" s="49">
         <v>1.2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Initial work on border tests.
</commit_message>
<xml_diff>
--- a/examples/styles/out.xlsx
+++ b/examples/styles/out.xlsx
@@ -371,68 +371,266 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
+      <diagonal/>
     </border>
     <border>
       <left style="thick"/>
       <right style="thick"/>
       <top style="thick"/>
       <bottom style="thick"/>
+      <diagonal/>
     </border>
     <border>
       <left>
-        <color rgb="ff0000"/>
+        <color rgb="FF0000"/>
       </left>
       <right style="thin">
-        <color rgb="ff0000"/>
+        <color rgb="FF0000"/>
       </right>
       <top>
-        <color rgb="ff0000"/>
+        <color rgb="FF0000"/>
       </top>
       <bottom>
-        <color rgb="ff0000"/>
+        <color rgb="FF0000"/>
       </bottom>
       <diagonal>
-        <color rgb="ff0000"/>
+        <color rgb="FF0000"/>
       </diagonal>
     </border>
     <border diagonalUp="1">
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal style="dashed">
         <color theme="6" tint="-0.1"/>
       </diagonal>
@@ -442,42 +640,104 @@
       <right style="thin"/>
       <top style="hair"/>
       <bottom style="medium"/>
+      <diagonal/>
     </border>
     <border>
       <left style="thick">
-        <color rgb="ffff00"/>
+        <color rgb="FFFF00"/>
       </left>
       <right style="thick">
-        <color rgb="00ff00"/>
+        <color rgb="00FF00"/>
       </right>
       <top style="thick">
-        <color rgb="ff0000"/>
+        <color rgb="FF0000"/>
       </top>
       <bottom style="thick">
-        <color rgb="0000ff"/>
+        <color rgb="0000FF"/>
       </bottom>
+      <diagonal/>
     </border>
     <border diagonalUp="1" diagonalDown="1">
       <left style="mediumDashed"/>
       <right style="thick"/>
       <top style="thin"/>
       <bottom style="dotted">
-        <color rgb="ff0000"/>
+        <color rgb="FF0000"/>
       </bottom>
       <diagonal style="thick">
-        <color rgb="0000ff"/>
+        <color rgb="0000FF"/>
       </diagonal>
     </border>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>

</xml_diff>

<commit_message>
Finished converting to JSON.
</commit_message>
<xml_diff>
--- a/examples/styles/out.xlsx
+++ b/examples/styles/out.xlsx
@@ -1125,10 +1125,6 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="25" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">

</xml_diff>